<commit_message>
improve the addr belongs q&a
</commit_message>
<xml_diff>
--- a/cbdb_llm_eval.xlsx
+++ b/cbdb_llm_eval.xlsx
@@ -448,79 +448,79 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>洪昕(c_personid=10159)的入仕方式是？</t>
+          <t>顏之義(c_personid=32425)的籍貫是？</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>恩蔭</t>
+          <t>長安</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>俞曰都(c_personid=374422)的籍貫是？</t>
+          <t>朱廷桂(c_personid=62740的籍貫是否為東都指揮使司？</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>鎮海衛</t>
+          <t>否</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>傅謙受(c_personid=11185)的入仕方式是？</t>
+          <t>袁國鳳(c_personid=655539的籍貫是否為為州？</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>恩蔭</t>
+          <t>否</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>孟釗(c_personid=348031)的入仕方式是？</t>
+          <t>王有壬(c_personid=34586)的入仕方式是？</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>進士</t>
+          <t>恩蔭</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>趙不驚(c_personid=19402)的籍貫是？</t>
+          <t>袁衡(c_personid=19396)的入仕方式是？</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>鄞縣</t>
+          <t>進士</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>嚴大翎(c_personid=597181)的籍貫是？</t>
+          <t>李虛舟(c_personid=3505)的入仕方式是？</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>廣東省</t>
+          <t>恩蔭</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>玉麟(c_personid=341512)的入仕方式是？</t>
+          <t>胡景定(c_personid=365873)的入仕方式是？</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>梁之材(c_personid=625424)的入仕方式是？</t>
+          <t>衝有雅(c_personid=655421)的入仕方式是？</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -544,19 +544,19 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>黃延詐(c_personid=681627)的籍貫是？</t>
+          <t>沈邦本(c_personid=632676的籍貫是否為寧州？</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>臺灣</t>
+          <t>否</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>夏在庭(c_personid=597521)的入仕方式是？</t>
+          <t>陳同熙(c_personid=669471)的入仕方式是？</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,67 +568,67 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>劉氏(江懋相妻)(c_personid=5410的籍貫是否為開封府？</t>
+          <t>陳大典(c_personid=371817)的入仕方式是？</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>是</t>
+          <t>進士</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>龍煥綸(c_personid=340143)的入仕方式是？</t>
+          <t>陳逸(c_personid=14542)的入仕方式是？</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>進士</t>
+          <t>恩蔭</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>莫廷芬(c_personid=541219)的入仕方式是？</t>
+          <t>劉伸(c_personid=557888的籍貫是否為陽州？</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>進士</t>
+          <t>否</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>焦沛霖(c_personid=634810的籍貫是否為奉天府？</t>
+          <t>陳邦光(c_personid=74)的入仕方式是？</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>是</t>
+          <t>進士</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>陳福臻(c_personid=671734)的入仕方式是？</t>
+          <t>單瑞龍(c_personid=368518)的籍貫是？</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>舉人</t>
+          <t>錢塘</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>蔣洪懿(c_personid=536710)的入仕方式是？</t>
+          <t>陸壑(c_personid=48095)的入仕方式是？</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -640,103 +640,103 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>趙士揆(c_personid=220631的籍貫是否為寧國府？</t>
+          <t>林叢桂(c_personid=624091)的入仕方式是？</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>是</t>
+          <t>舉人</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>趙鴻謀(c_personid=661568的籍貫是否為紹興府？</t>
+          <t>李有普(c_personid=620769)的入仕方式是？</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>是</t>
+          <t>恩蔭</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>李延興(c_personid=28648的籍貫是否為順天府？</t>
+          <t>王文烱(c_personid=327293的籍貫是否為平州？</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>是</t>
+          <t>否</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>黃嘉(c_personid=34537)的籍貫是？</t>
+          <t>舒嘉猷(c_personid=90244的籍貫是否為慶州？</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>莆田</t>
+          <t>否</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>鄭弘勣(c_personid=191359)的籍貫是？</t>
+          <t>徐淮(c_personid=385952)的入仕方式是？</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>福州</t>
+          <t>進士</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>楊潮宗(c_personid=287149的籍貫是否為武昌府？</t>
+          <t>張公邵(c_personid=26542)的入仕方式是？</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>是</t>
+          <t>恩蔭</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>俞世德(c_personid=200546)的籍貫是？</t>
+          <t>周春(c_personid=33209的籍貫是否為寧州？</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>無錫</t>
+          <t>否</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>高載銘(c_personid=678779)的入仕方式是？</t>
+          <t>王杲(c_personid=39477)的籍貫是？</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>舉人</t>
+          <t>齊州</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>張椿蔭(c_personid=607717)的入仕方式是？</t>
+          <t>胡永榮(c_personid=648279)的入仕方式是？</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -748,31 +748,31 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>王選衆(c_personid=640403)的入仕方式是？</t>
+          <t>呂弼康(c_personid=43017)的籍貫是？</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>舉人</t>
+          <t>餘干</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>王萬邦(c_personid=57202)的籍貫是？</t>
+          <t>易俊(c_personid=59256的籍貫是否為國州？</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>陽高</t>
+          <t>否</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>陳彥先(c_personid=15068)的入仕方式是？</t>
+          <t>徐子端(c_personid=27782)的入仕方式是？</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -784,67 +784,67 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>張奎光(c_personid=346192)的入仕方式是？</t>
+          <t>包景寧(c_personid=589572)的入仕方式是？</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>進士</t>
+          <t>舉人</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>姚克濬(c_personid=597918的籍貫是否為杭州府？</t>
+          <t>劉運隆(c_personid=369916)的入仕方式是？</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>是</t>
+          <t>進士</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>何蔭垣(c_personid=582307的籍貫是否為鳳翔府？</t>
+          <t>王鵬運(c_personid=54979)的入仕方式是？</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>是</t>
+          <t>舉人</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>楊襄(c_personid=28359)的入仕方式是？</t>
+          <t>胡鶴(c_personid=300994)的籍貫是？</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>恩蔭</t>
+          <t>歙縣</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>周宗起(c_personid=373015)的入仕方式是？</t>
+          <t>陳徽言(c_personid=82250的籍貫是否為川州？</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>進士</t>
+          <t>否</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>陳燕泰(c_personid=671500)的入仕方式是？</t>
+          <t>孔羲仲(c_personid=126186)的入仕方式是？</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -856,7 +856,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>陳時南(c_personid=670886)的入仕方式是？</t>
+          <t>陳宗鳳(c_personid=670003)的入仕方式是？</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -868,31 +868,31 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>馬體咸(c_personid=677058)的入仕方式是？</t>
+          <t>某徵(c_personid=555494)的入仕方式是？</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>舉人</t>
+          <t>進士</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>蕭俶(c_personid=33114)的入仕方式是？</t>
+          <t>劉廷聞(c_personid=586841)的入仕方式是？</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>恩蔭</t>
+          <t>舉人</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>魯逢甲(c_personid=679664)的入仕方式是？</t>
+          <t>張淑躬(c_personid=608044)的入仕方式是？</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -904,7 +904,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>孫尚紱(c_personid=599965)的入仕方式是？</t>
+          <t>李名瑚(c_personid=618707)的入仕方式是？</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -916,31 +916,31 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>韓瑄(c_personid=17724)的入仕方式是？</t>
+          <t>尹光楨(c_personid=602462)的籍貫是？</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>恩蔭</t>
+          <t>新城</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>張誼(c_personid=204200的籍貫是否為紹興府？</t>
+          <t>程再伊(c_personid=559998)的籍貫是？</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>是</t>
+          <t>鄱陽</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>楊崇勳(c_personid=1997)的入仕方式是？</t>
+          <t>吳公瑾(c_personid=593506)的入仕方式是？</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -952,96 +952,96 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>赫望嵋(c_personid=659738)的籍貫是？</t>
+          <t>辛本婺(c_personid=661823)的籍貫是？</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>文昌</t>
+          <t>蓬萊</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>胡居仁(c_personid=42989)的入仕方式是？</t>
+          <t>蔡雲吉(c_personid=493073)的入仕方式是？</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>進士</t>
+          <t>舉人</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>吉明(c_personid=359562)的入仕方式是？</t>
+          <t>胡實(c_personid=11871)的入仕方式是？</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>進士</t>
+          <t>恩蔭</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>靳大文(c_personid=674270)的籍貫是？</t>
+          <t>張曾垿(c_personid=347008)的入仕方式是？</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>介休</t>
+          <t>進士</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>鄭億年(c_personid=15274的籍貫是否為開封府？</t>
+          <t>吳秉翰(c_personid=592604的籍貫是否為平府直轄地方？</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>是</t>
+          <t>否</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>徐士豪(c_personid=611146)的入仕方式是？</t>
+          <t>陳成務(c_personid=541971)的籍貫是？</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>恩蔭</t>
+          <t>晉江</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>傅貴早(c_personid=531984)的入仕方式是？</t>
+          <t>石萬寶(c_personid=643103)的籍貫是？</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>進士</t>
+          <t>如皋</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>廖簡(c_personid=557005)的入仕方式是？</t>
+          <t>松壽(c_personid=366024)的入仕方式是？</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>舉人</t>
+          <t>進士</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
improve the addr belong q&a
</commit_message>
<xml_diff>
--- a/cbdb_llm_eval.xlsx
+++ b/cbdb_llm_eval.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,103 +448,103 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>顏之義(c_personid=32425)的籍貫是？</t>
+          <t>馬際泰(c_personid=677027)的入仕方式是？</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>長安</t>
+          <t>舉人</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>朱廷桂(c_personid=62740的籍貫是否為東都指揮使司？</t>
+          <t>夏錫金(c_personid=344371)的入仕方式是？</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>否</t>
+          <t>進士</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>袁國鳳(c_personid=655539的籍貫是否為為州？</t>
+          <t>鍾德浦(c_personid=667675)的入仕方式是？</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>否</t>
+          <t>恩蔭</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>王有壬(c_personid=34586)的入仕方式是？</t>
+          <t>悟勤善淳(c_personid=375984)的入仕方式是？</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>恩蔭</t>
+          <t>進士</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>袁衡(c_personid=19396)的入仕方式是？</t>
+          <t>陳錡(c_personid=124113的籍貫是否為郵州？</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>進士</t>
+          <t>否</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>李虛舟(c_personid=3505)的入仕方式是？</t>
+          <t>王禹功(c_personid=342115)的入仕方式是？</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>恩蔭</t>
+          <t>進士</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>胡景定(c_personid=365873)的入仕方式是？</t>
+          <t>展毓(c_personid=198547的籍貫是否為騎右衛？</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>進士</t>
+          <t>否</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>衝有雅(c_personid=655421)的入仕方式是？</t>
+          <t>潘之驤(c_personid=634068)的籍貫是？</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>舉人</t>
+          <t>仁和</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>沈邦本(c_personid=632676的籍貫是否為寧州？</t>
+          <t>盧庭琮(c_personid=348921的籍貫是否為國州？</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -556,307 +556,307 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>陳同熙(c_personid=669471)的入仕方式是？</t>
+          <t>程天秩(c_personid=7135)的入仕方式是？</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>舉人</t>
+          <t>恩蔭</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>陳大典(c_personid=371817)的入仕方式是？</t>
+          <t>吳洵武(c_personid=27040)的入仕方式是？</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>進士</t>
+          <t>舉人</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>陳逸(c_personid=14542)的入仕方式是？</t>
+          <t>陳錡(c_personid=124113的籍貫是否為揚州府？</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>恩蔭</t>
+          <t>是</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>劉伸(c_personid=557888的籍貫是否為陽州？</t>
+          <t>謝顯光(c_personid=658370)的入仕方式是？</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>否</t>
+          <t>恩蔭</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>陳邦光(c_personid=74)的入仕方式是？</t>
+          <t>栗寬(c_personid=625265的籍貫是否為源州？</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>進士</t>
+          <t>否</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>單瑞龍(c_personid=368518)的籍貫是？</t>
+          <t>袁世承(c_personid=655454)的入仕方式是？</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>錢塘</t>
+          <t>恩蔭</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>陸壑(c_personid=48095)的入仕方式是？</t>
+          <t>楊玉山(c_personid=118508)的籍貫是？</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>進士</t>
+          <t>松江府</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>林叢桂(c_personid=624091)的入仕方式是？</t>
+          <t>沈文明(c_personid=223855的籍貫是否為蘇州府？</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>舉人</t>
+          <t>是</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>李有普(c_personid=620769)的入仕方式是？</t>
+          <t>童榮(c_personid=248616)的籍貫是？</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>恩蔭</t>
+          <t>蘭溪</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>王文烱(c_personid=327293的籍貫是否為平州？</t>
+          <t>胡永華(c_personid=648284)的籍貫是？</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>否</t>
+          <t>懷寧</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>舒嘉猷(c_personid=90244的籍貫是否為慶州？</t>
+          <t>王稷(c_personid=189639)的籍貫是？</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>否</t>
+          <t>河中府</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>徐淮(c_personid=385952)的入仕方式是？</t>
+          <t>張經(c_personid=320803的籍貫是否為揚州府？</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>進士</t>
+          <t>是</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>張公邵(c_personid=26542)的入仕方式是？</t>
+          <t>袁一鰲(c_personid=550662)的入仕方式是？</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>恩蔭</t>
+          <t>舉人</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>周春(c_personid=33209的籍貫是否為寧州？</t>
+          <t>徐紹心(c_personid=319410)的籍貫是？</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>否</t>
+          <t>餘姚</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>王杲(c_personid=39477)的籍貫是？</t>
+          <t>夏士錦(c_personid=344320)的入仕方式是？</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>齊州</t>
+          <t>進士</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>胡永榮(c_personid=648279)的入仕方式是？</t>
+          <t>樊廷茂(c_personid=44998)的入仕方式是？</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>舉人</t>
+          <t>進士</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>呂弼康(c_personid=43017)的籍貫是？</t>
+          <t>嚴一介(c_personid=597117)的入仕方式是？</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>餘干</t>
+          <t>舉人</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>易俊(c_personid=59256的籍貫是否為國州？</t>
+          <t>胡順(c_personid=34481)的入仕方式是？</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>否</t>
+          <t>恩蔭</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>徐子端(c_personid=27782)的入仕方式是？</t>
+          <t>張經(c_personid=320803的籍貫是否為郵州？</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>恩蔭</t>
+          <t>否</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>包景寧(c_personid=589572)的入仕方式是？</t>
+          <t>徐榕(c_personid=13035)的入仕方式是？</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>舉人</t>
+          <t>恩蔭</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>劉運隆(c_personid=369916)的入仕方式是？</t>
+          <t>盧庭琮(c_personid=348921的籍貫是否為武昌府？</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>進士</t>
+          <t>是</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>王鵬運(c_personid=54979)的入仕方式是？</t>
+          <t>王綺珍(c_personid=342339的籍貫是否為臨安府？</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>舉人</t>
+          <t>是</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>胡鶴(c_personid=300994)的籍貫是？</t>
+          <t>周熙有(c_personid=595264)的入仕方式是？</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>歙縣</t>
+          <t>舉人</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>陳徽言(c_personid=82250的籍貫是否為川州？</t>
+          <t>趙希府(c_personid=536746)的入仕方式是？</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>否</t>
+          <t>進士</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>孔羲仲(c_personid=126186)的入仕方式是？</t>
+          <t>戴洪緒(c_personid=613079)的入仕方式是？</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>恩蔭</t>
+          <t>舉人</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>陳宗鳳(c_personid=670003)的入仕方式是？</t>
+          <t>彭萬涵(c_personid=610647)的入仕方式是？</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -868,180 +868,300 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>某徵(c_personid=555494)的入仕方式是？</t>
+          <t>陳鳳廷(c_personid=672711)的入仕方式是？</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>進士</t>
+          <t>舉人</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>劉廷聞(c_personid=586841)的入仕方式是？</t>
+          <t>王珝(c_personid=342024的籍貫是否為平衛？</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>舉人</t>
+          <t>否</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>張淑躬(c_personid=608044)的入仕方式是？</t>
+          <t>劉錡(c_personid=24320)的入仕方式是？</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>舉人</t>
+          <t>恩蔭</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>李名瑚(c_personid=618707)的入仕方式是？</t>
+          <t>胡汝瀾(c_personid=648294的籍貫是否為陰廳？</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>恩蔭</t>
+          <t>否</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>尹光楨(c_personid=602462)的籍貫是？</t>
+          <t>譚顯相(c_personid=340256)的入仕方式是？</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>新城</t>
+          <t>進士</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>程再伊(c_personid=559998)的籍貫是？</t>
+          <t>耿承祖(c_personid=105844)的入仕方式是？</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>鄱陽</t>
+          <t>恩蔭</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>吳公瑾(c_personid=593506)的入仕方式是？</t>
+          <t>龔聞道(c_personid=206928的籍貫是否為倉州？</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>恩蔭</t>
+          <t>否</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>辛本婺(c_personid=661823)的籍貫是？</t>
+          <t>齊棟(c_personid=682450)的入仕方式是？</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>蓬萊</t>
+          <t>舉人</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>蔡雲吉(c_personid=493073)的入仕方式是？</t>
+          <t>衛璜書(c_personid=655388)的籍貫是？</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>舉人</t>
+          <t>趙城</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>胡實(c_personid=11871)的入仕方式是？</t>
+          <t>展毓(c_personid=198547的籍貫是否為右軍都督府？</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>恩蔭</t>
+          <t>是</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>張曾垿(c_personid=347008)的入仕方式是？</t>
+          <t>張翕(c_personid=346964)的籍貫是？</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>進士</t>
+          <t>山東省</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>吳秉翰(c_personid=592604的籍貫是否為平府直轄地方？</t>
+          <t>張燾(c_personid=64240)的入仕方式是？</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>否</t>
+          <t>進士</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>陳成務(c_personid=541971)的籍貫是？</t>
+          <t>胡汝瀾(c_personid=648294的籍貫是否為興安府？</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>晉江</t>
+          <t>是</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>石萬寶(c_personid=643103)的籍貫是？</t>
+          <t>王珝(c_personid=342024的籍貫是否為後軍都督府？</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>如皋</t>
+          <t>是</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>松壽(c_personid=366024)的入仕方式是？</t>
+          <t>沈文明(c_personid=223855的籍貫是否為倉州？</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
+          <t>否</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>龔聞道(c_personid=206928的籍貫是否為蘇州府？</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>是</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>蔡名載(c_personid=363279)的入仕方式是？</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
           <t>進士</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>沈修文(c_personid=631676)的入仕方式是？</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>舉人</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>葉得榕(c_personid=651043)的籍貫是？</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>湖南省</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>唐拱(c_personid=3829)的入仕方式是？</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>恩蔭</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>王廣廉(c_personid=1843)的籍貫是？</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>洹水</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>栗寬(c_personid=625265的籍貫是否為大同府？</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>是</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>南宮鼎(c_personid=357302)的入仕方式是？</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>進士</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>王綺珍(c_personid=342339的籍貫是否為屏州？</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>否</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>裴冕(c_personid=32838)的入仕方式是？</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>恩蔭</t>
         </is>
       </c>
     </row>

</xml_diff>